<commit_message>
indo para API COMPRASGOV
</commit_message>
<xml_diff>
--- a/DOWNLOADS/livro_razao.xlsx
+++ b/DOWNLOADS/livro_razao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="371">
   <si>
     <t>Timestamp</t>
   </si>
@@ -37,7 +37,19 @@
     <t>Link Compras.gov</t>
   </si>
   <si>
-    <t>2025-09-06 14:22:35</t>
+    <t>2025-09-07 09:47:00</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:07:58</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:30:18</t>
+  </si>
+  <si>
+    <t>2025-09-08 14:48:50</t>
+  </si>
+  <si>
+    <t>2025-09-08 15:45:03</t>
   </si>
   <si>
     <t>18/09/2025 - 09:00</t>
@@ -145,15 +157,27 @@
     <t>09/09/2025 - 09:00</t>
   </si>
   <si>
+    <t>09/09/2025 - 10:00</t>
+  </si>
+  <si>
     <t>11/09/2025 - 16:00</t>
   </si>
   <si>
-    <t>09/09/2025 - 10:00</t>
-  </si>
-  <si>
     <t>08/09/2025 - 09:00</t>
   </si>
   <si>
+    <t>29/09/2025 - 09:00</t>
+  </si>
+  <si>
+    <t>23/09/2025 - 09:00</t>
+  </si>
+  <si>
+    <t>15/09/2025 - 10:30</t>
+  </si>
+  <si>
+    <t>08/09/2025 - 08:30</t>
+  </si>
+  <si>
     <t>927317</t>
   </si>
   <si>
@@ -337,6 +361,9 @@
     <t>929994</t>
   </si>
   <si>
+    <t>160237</t>
+  </si>
+  <si>
     <t>179087</t>
   </si>
   <si>
@@ -367,6 +394,45 @@
     <t>986843</t>
   </si>
   <si>
+    <t>153019</t>
+  </si>
+  <si>
+    <t>927190</t>
+  </si>
+  <si>
+    <t>928576</t>
+  </si>
+  <si>
+    <t>157249</t>
+  </si>
+  <si>
+    <t>453330</t>
+  </si>
+  <si>
+    <t>102150</t>
+  </si>
+  <si>
+    <t>982929</t>
+  </si>
+  <si>
+    <t>180196</t>
+  </si>
+  <si>
+    <t>453747</t>
+  </si>
+  <si>
+    <t>160251</t>
+  </si>
+  <si>
+    <t>158456</t>
+  </si>
+  <si>
+    <t>160441</t>
+  </si>
+  <si>
+    <t>160363</t>
+  </si>
+  <si>
     <t>900342025</t>
   </si>
   <si>
@@ -526,6 +592,18 @@
     <t>900292025</t>
   </si>
   <si>
+    <t>900862025</t>
+  </si>
+  <si>
+    <t>902292025</t>
+  </si>
+  <si>
+    <t>900022025</t>
+  </si>
+  <si>
+    <t>900062025</t>
+  </si>
+  <si>
     <t>SERVIÇO AUTÔNOMO DE ÁGUA E ESGOTO DE ITAUNA</t>
   </si>
   <si>
@@ -709,6 +787,9 @@
     <t>CÂMARA MUNICIPAL DE SAO LUIZ GONZAGA/RS</t>
   </si>
   <si>
+    <t>MINISTÉRIO DA DEFESA / Comando do Exército / Secretaria de Ciência e Tecnologia / Centro Tecnológico do Exército / Centro de Avaliação do Exército</t>
+  </si>
+  <si>
     <t>MINISTÉRIO DA ECONOMIA / BANCO CENTRAL DO BRASIL / Diretoria de Administração - DIRAD / Departamento de Infraestrutura e Gestão Patrimonial - DEMAP</t>
   </si>
   <si>
@@ -739,6 +820,45 @@
     <t>PREF.MUN.DE PEDREIRA</t>
   </si>
   <si>
+    <t>MINISTÉRIO DA EDUCAÇÃO / Universidade Tecnológica Federal do Paraná</t>
+  </si>
+  <si>
+    <t>Governo do Estado de Mato Grosso / SERVIÇO DE SANEAMENTO AMBIENTAL ÁGUAS DO PANTANAL</t>
+  </si>
+  <si>
+    <t>SERVIÇO AUTONOMO MUNICIPAL DE AGUA E ESGOTO</t>
+  </si>
+  <si>
+    <t>MINISTÉRIO DA EDUCAÇÃO / Hospital Universitário da Universidade Federal de Roraima</t>
+  </si>
+  <si>
+    <t>PREFEITURA DA ESTANCIA HIDROMINERAL DE POA ESTADO DE SAO PAULO</t>
+  </si>
+  <si>
+    <t>GOVERNO DO ESTADO DE SÃO PAULO / ESP-SECRETARIA DE CIENCIA TECNOL E INOVAÇÃO / ESP-HOSPITAL UNIVERSITÁRIO - USP</t>
+  </si>
+  <si>
+    <t>Prefeitura Municipal de Marechal Floriano/ES</t>
+  </si>
+  <si>
+    <t>GOVERNO DO ESTADO DE SÃO PAULO / ESP-SECRETARIA DA SEGURANCA PUBLICA / ESP-COMANDO DE POLICIAMENTO DE TRANSITO</t>
+  </si>
+  <si>
+    <t>Governo do Estado do Maranhão / DEFENSORIA PUBLICA DO ESTADO MARANHÃO</t>
+  </si>
+  <si>
+    <t>MINISTÉRIO DA DEFESA / Comando do Exército / Comando Militar do Leste / 1ªDivisão de Exército / GUEs/9ªBrigada de Infantaria Motorizada / Batalhao Escola de Comunicações</t>
+  </si>
+  <si>
+    <t>MINISTÉRIO DA EDUCAÇÃO / Secretaria Executiva / Subsecretaria de Planejamento e Orçamento / Instituto Federal de Educação, Ciência e Tecnologia do Maranhão / Campus Caxias</t>
+  </si>
+  <si>
+    <t>MINISTÉRIO DA DEFESA / Comando do Exército / Comando Militar do Sul / 5ª Região Militar / 14ªBrigada de Infantaria Motorizada / 28ºGrupo de Artilharia de Campanha</t>
+  </si>
+  <si>
+    <t>MINISTÉRIO DA DEFESA / Comando do Exército / Comando Militar do Sul / 6ªDivisão de Exército / 3ªBrigada de Cavalaria Mecanizada / 3ºRegimento de Cavalaria Mecanizado</t>
+  </si>
+  <si>
     <t>U_927317_E_900342025_C_SERVIÇO_AUTÔNOMO_DE_ÁGUA_E_ESGOTO_DE_ITAUNA_18-09-2025_09h00m.zip</t>
   </si>
   <si>
@@ -928,6 +1048,9 @@
     <t>U_929994_E_900042025_C_CÂMARA_MUNICIPAL_DE_SAO_LUIZ_GONZAGA_RS_09-09-2025_09h00m.zip</t>
   </si>
   <si>
+    <t>U_160237_E_900082025_C_MINISTÉRIO_DA_DEFESA___Comando_do_Exército___Secretaria_de_Ciência_e_Tecnologia___Centro_Tecnológico_do_Exército___Centro_de_Avaliação_do_Exército_09-09-2025_10h00m.zip</t>
+  </si>
+  <si>
     <t>U_179087_E_900602025_C_MINISTÉRIO_DA_ECONOMIA___BANCO_CENTRAL_DO_BRASIL___Diretoria_de_Administração_-_DIRAD___Departamento_de_Infraestrutura_e_Gestão_Patrimonial_-_DEMAP_11-09-2025_16h00m.zip</t>
   </si>
   <si>
@@ -959,6 +1082,51 @@
   </si>
   <si>
     <t>U_986843_E_900262025_C_PREF_MUN_DE_PEDREIRA_10-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_153019_E_900092025_18-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_927190_E_900142025_17-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_928576_E_900862025_29-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_157249_E_900032025_17-09-2025_10h00m.zip</t>
+  </si>
+  <si>
+    <t>U_453330_E_900432025_19-09-2025_10h00m.zip</t>
+  </si>
+  <si>
+    <t>U_986843_E_900292025_18-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_102328_E_900132025_18-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_102150_E_902292025_18-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_982929_E_900032025_17-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_180196_E_900262025_18-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_453747_E_900282025_23-09-2025_09h00m.zip</t>
+  </si>
+  <si>
+    <t>U_160251_E_900022025_11-09-2025_08h00m.zip</t>
+  </si>
+  <si>
+    <t>U_158456_E_900032025_15-09-2025_08h00m.zip</t>
+  </si>
+  <si>
+    <t>U_160441_E_900082025_15-09-2025_10h30m.zip</t>
+  </si>
+  <si>
+    <t>U_160363_E_900062025_08-09-2025_08h30m.zip</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1484,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1350,19 +1518,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="F2" t="s">
-        <v>241</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1370,19 +1538,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="F3" t="s">
-        <v>242</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1390,19 +1558,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="E4" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="F4" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1410,19 +1578,19 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="F5" t="s">
-        <v>244</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1430,19 +1598,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="F6" t="s">
-        <v>245</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1450,19 +1618,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="E7" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1470,19 +1638,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>247</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1490,19 +1658,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="F9" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1510,19 +1678,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
       <c r="F10" t="s">
-        <v>249</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1530,19 +1698,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="F11" t="s">
-        <v>250</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1550,19 +1718,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="F12" t="s">
-        <v>251</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1570,19 +1738,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1590,19 +1758,19 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="F14" t="s">
-        <v>253</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1610,19 +1778,19 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="E15" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="F15" t="s">
-        <v>254</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1630,19 +1798,19 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>255</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1650,19 +1818,19 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
       <c r="F17" t="s">
-        <v>256</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1670,19 +1838,19 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1690,19 +1858,19 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
       <c r="F19" t="s">
-        <v>258</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1710,19 +1878,19 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="E20" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
       <c r="F20" t="s">
-        <v>259</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1730,19 +1898,19 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="F21" t="s">
-        <v>260</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1750,19 +1918,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="E22" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="F22" t="s">
-        <v>261</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1770,19 +1938,19 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="F23" t="s">
-        <v>262</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1790,19 +1958,19 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="E24" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="F24" t="s">
-        <v>263</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1810,19 +1978,19 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
       <c r="F25" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1830,19 +1998,19 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
       <c r="F26" t="s">
-        <v>265</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1850,19 +2018,19 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="E27" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="F27" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1870,19 +2038,19 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
       <c r="F28" t="s">
-        <v>267</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1890,19 +2058,19 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="E29" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
       <c r="F29" t="s">
-        <v>268</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1910,19 +2078,19 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="F30" t="s">
-        <v>269</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1930,19 +2098,19 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="E31" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="F31" t="s">
-        <v>270</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1950,19 +2118,19 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E32" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="F32" t="s">
-        <v>271</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1970,19 +2138,19 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="E33" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="F33" t="s">
-        <v>272</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1990,19 +2158,19 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="F34" t="s">
-        <v>273</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2010,19 +2178,19 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="E35" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
       <c r="F35" t="s">
-        <v>274</v>
+        <v>314</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2030,19 +2198,19 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="E36" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
       <c r="F36" t="s">
-        <v>275</v>
+        <v>315</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2050,19 +2218,19 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E37" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
       <c r="F37" t="s">
-        <v>276</v>
+        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2070,19 +2238,19 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="E38" t="s">
-        <v>205</v>
+        <v>231</v>
       </c>
       <c r="F38" t="s">
-        <v>277</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2090,19 +2258,19 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="E39" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="F39" t="s">
-        <v>278</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2110,19 +2278,19 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
       <c r="F40" t="s">
-        <v>279</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2130,19 +2298,19 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="F41" t="s">
-        <v>280</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2150,19 +2318,19 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="E42" t="s">
-        <v>209</v>
+        <v>235</v>
       </c>
       <c r="F42" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -2170,19 +2338,19 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="E43" t="s">
-        <v>210</v>
+        <v>236</v>
       </c>
       <c r="F43" t="s">
-        <v>282</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2190,19 +2358,19 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="E44" t="s">
-        <v>211</v>
+        <v>237</v>
       </c>
       <c r="F44" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2210,19 +2378,19 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="E45" t="s">
-        <v>212</v>
+        <v>238</v>
       </c>
       <c r="F45" t="s">
-        <v>284</v>
+        <v>324</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2230,19 +2398,19 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E46" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="F46" t="s">
-        <v>285</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -2250,19 +2418,19 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="F47" t="s">
-        <v>286</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2270,19 +2438,19 @@
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="F48" t="s">
-        <v>287</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2290,19 +2458,19 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="F49" t="s">
-        <v>288</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2310,19 +2478,19 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="F50" t="s">
-        <v>289</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2330,19 +2498,19 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="E51" t="s">
-        <v>218</v>
+        <v>244</v>
       </c>
       <c r="F51" t="s">
-        <v>290</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2350,19 +2518,19 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="E52" t="s">
-        <v>219</v>
+        <v>245</v>
       </c>
       <c r="F52" t="s">
-        <v>291</v>
+        <v>331</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2370,19 +2538,19 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="E53" t="s">
-        <v>220</v>
+        <v>246</v>
       </c>
       <c r="F53" t="s">
-        <v>292</v>
+        <v>332</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2390,19 +2558,19 @@
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="E54" t="s">
-        <v>181</v>
+        <v>207</v>
       </c>
       <c r="F54" t="s">
-        <v>293</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2410,19 +2578,19 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="E55" t="s">
-        <v>221</v>
+        <v>247</v>
       </c>
       <c r="F55" t="s">
-        <v>294</v>
+        <v>334</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2430,19 +2598,19 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D56" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="E56" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
       <c r="F56" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2450,19 +2618,19 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="E57" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="F57" t="s">
-        <v>296</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2470,19 +2638,19 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D58" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="E58" t="s">
-        <v>224</v>
+        <v>250</v>
       </c>
       <c r="F58" t="s">
-        <v>297</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2490,19 +2658,19 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E59" t="s">
-        <v>225</v>
+        <v>251</v>
       </c>
       <c r="F59" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2510,19 +2678,19 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D60" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
-        <v>226</v>
+        <v>252</v>
       </c>
       <c r="F60" t="s">
-        <v>299</v>
+        <v>339</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2530,19 +2698,19 @@
         <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="D61" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="E61" t="s">
-        <v>227</v>
+        <v>253</v>
       </c>
       <c r="F61" t="s">
-        <v>300</v>
+        <v>340</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2550,19 +2718,19 @@
         <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="E62" t="s">
-        <v>228</v>
+        <v>254</v>
       </c>
       <c r="F62" t="s">
-        <v>301</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2570,19 +2738,19 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="E63" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="F63" t="s">
-        <v>302</v>
+        <v>342</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -2590,19 +2758,19 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="F64" t="s">
-        <v>303</v>
+        <v>343</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2610,19 +2778,19 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C65" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D65" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E65" t="s">
-        <v>231</v>
+        <v>257</v>
       </c>
       <c r="F65" t="s">
-        <v>304</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -2630,19 +2798,19 @@
         <v>7</v>
       </c>
       <c r="B66" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D66" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="E66" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="F66" t="s">
-        <v>305</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2650,19 +2818,19 @@
         <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D67" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="E67" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="F67" t="s">
-        <v>306</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -2670,19 +2838,19 @@
         <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C68" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D68" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="E68" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
       <c r="F68" t="s">
-        <v>307</v>
+        <v>347</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -2690,19 +2858,19 @@
         <v>7</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="E69" t="s">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="F69" t="s">
-        <v>308</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2710,19 +2878,19 @@
         <v>7</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D70" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="E70" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="F70" t="s">
-        <v>309</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2730,19 +2898,19 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D71" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="E71" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
       <c r="F71" t="s">
-        <v>310</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2750,19 +2918,19 @@
         <v>7</v>
       </c>
       <c r="B72" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C72" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="D72" t="s">
-        <v>117</v>
+        <v>190</v>
       </c>
       <c r="E72" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="F72" t="s">
-        <v>311</v>
+        <v>351</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2770,19 +2938,19 @@
         <v>7</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C73" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D73" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="E73" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="F73" t="s">
-        <v>312</v>
+        <v>352</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2790,19 +2958,19 @@
         <v>7</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C74" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E74" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
       <c r="F74" t="s">
-        <v>313</v>
+        <v>353</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2810,19 +2978,339 @@
         <v>7</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D75" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="E75" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="F75" t="s">
-        <v>314</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76" t="s">
+        <v>144</v>
+      </c>
+      <c r="E76" t="s">
+        <v>267</v>
+      </c>
+      <c r="F76" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" t="s">
+        <v>126</v>
+      </c>
+      <c r="D77" t="s">
+        <v>162</v>
+      </c>
+      <c r="E77" t="s">
+        <v>268</v>
+      </c>
+      <c r="F77" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" t="s">
+        <v>179</v>
+      </c>
+      <c r="E78" t="s">
+        <v>269</v>
+      </c>
+      <c r="F78" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s">
+        <v>128</v>
+      </c>
+      <c r="D79" t="s">
+        <v>192</v>
+      </c>
+      <c r="E79" t="s">
+        <v>270</v>
+      </c>
+      <c r="F79" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>129</v>
+      </c>
+      <c r="D80" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" t="s">
+        <v>271</v>
+      </c>
+      <c r="F80" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" t="s">
+        <v>10</v>
+      </c>
+      <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" t="s">
+        <v>130</v>
+      </c>
+      <c r="D81" t="s">
+        <v>183</v>
+      </c>
+      <c r="E81" t="s">
+        <v>272</v>
+      </c>
+      <c r="F81" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" t="s">
+        <v>10</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>125</v>
+      </c>
+      <c r="D82" t="s">
+        <v>191</v>
+      </c>
+      <c r="E82" t="s">
+        <v>267</v>
+      </c>
+      <c r="F82" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B83" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83" t="s">
+        <v>172</v>
+      </c>
+      <c r="E83" t="s">
+        <v>266</v>
+      </c>
+      <c r="F83" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>11</v>
+      </c>
+      <c r="B84" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" t="s">
+        <v>131</v>
+      </c>
+      <c r="D84" t="s">
+        <v>193</v>
+      </c>
+      <c r="E84" t="s">
+        <v>273</v>
+      </c>
+      <c r="F84" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" t="s">
+        <v>132</v>
+      </c>
+      <c r="D85" t="s">
+        <v>166</v>
+      </c>
+      <c r="E85" t="s">
+        <v>274</v>
+      </c>
+      <c r="F85" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D86" t="s">
+        <v>144</v>
+      </c>
+      <c r="E86" t="s">
+        <v>275</v>
+      </c>
+      <c r="F86" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" t="s">
+        <v>134</v>
+      </c>
+      <c r="D87" t="s">
+        <v>143</v>
+      </c>
+      <c r="E87" t="s">
+        <v>276</v>
+      </c>
+      <c r="F87" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D88" t="s">
+        <v>194</v>
+      </c>
+      <c r="E88" t="s">
+        <v>277</v>
+      </c>
+      <c r="F88" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" t="s">
+        <v>136</v>
+      </c>
+      <c r="D89" t="s">
+        <v>166</v>
+      </c>
+      <c r="E89" t="s">
+        <v>278</v>
+      </c>
+      <c r="F89" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" t="s">
+        <v>11</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D90" t="s">
+        <v>156</v>
+      </c>
+      <c r="E90" t="s">
+        <v>279</v>
+      </c>
+      <c r="F90" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" t="s">
+        <v>138</v>
+      </c>
+      <c r="D91" t="s">
+        <v>195</v>
+      </c>
+      <c r="E91" t="s">
+        <v>280</v>
+      </c>
+      <c r="F91" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>